<commit_message>
0.2 version: support nested workflow
</commit_message>
<xml_diff>
--- a/src/config/config.xlsx
+++ b/src/config/config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="6930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -64,19 +64,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Robot 1: Excute all your test cases</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Robot 2: Excute just one test case (you pickup later)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Robot 4: Check code standards</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Please choose which sub-robot you want to excute</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -374,6 +362,18 @@
   </si>
   <si>
     <t>{0} [{1}] - case [{2}] tested result: {3}</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Robot 1: Execute all your test cases</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Robot 2: Execute just one test case (you pickup later)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Please choose which sub-robot you want to execute</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -808,8 +808,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -832,13 +832,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -846,74 +846,74 @@
         <v>3</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A7" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A8" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B8" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B9" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
@@ -921,18 +921,18 @@
         <v>8</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11" s="12"/>
     </row>
@@ -947,24 +947,24 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
@@ -972,17 +972,17 @@
         <v>7</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
@@ -1185,8 +1185,8 @@
   </sheetPr>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1209,46 +1209,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -1257,142 +1257,142 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C22" s="2"/>
     </row>
@@ -1412,7 +1412,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1435,28 +1435,28 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>82</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="C4" s="2"/>
     </row>

</xml_diff>